<commit_message>
update the timetable parser and week comparer
</commit_message>
<xml_diff>
--- a/src/test/resources/timetable-parser/timetable-0.xlsx
+++ b/src/test/resources/timetable-parser/timetable-0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eqour\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eqour\IdeaProjects\timetable-notifier\src\test\resources\timetable-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="24.10.2022-29.10.2022" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="61">
-  <si>
-    <t>24.10.2022</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="55">
   <si>
     <t>8:20-9:50</t>
   </si>
@@ -60,9 +57,6 @@
     <t>18:50-20:20</t>
   </si>
   <si>
-    <t>25.10.2022</t>
-  </si>
-  <si>
     <t>18:30-18:45</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>https://mirapolis.ru</t>
   </si>
   <si>
-    <t>26.10.2022</t>
-  </si>
-  <si>
     <t>Основы банковского дела</t>
   </si>
   <si>
@@ -96,12 +87,6 @@
     <t>14/1</t>
   </si>
   <si>
-    <t>27.10.2022</t>
-  </si>
-  <si>
-    <t>28.10.2022</t>
-  </si>
-  <si>
     <t>Информационные технологии поддержки принятия решений</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>13/1</t>
   </si>
   <si>
-    <t>29.10.2022</t>
-  </si>
-  <si>
     <t>Проектирование информационных систем</t>
   </si>
   <si>
@@ -129,24 +111,6 @@
     <t>21/1</t>
   </si>
   <si>
-    <t>31.10.2022</t>
-  </si>
-  <si>
-    <t>01.11.2022</t>
-  </si>
-  <si>
-    <t>02.11.2022</t>
-  </si>
-  <si>
-    <t>03.11.2022</t>
-  </si>
-  <si>
-    <t>04.11.2022</t>
-  </si>
-  <si>
-    <t>05.11.2022</t>
-  </si>
-  <si>
     <t>ОБ-Вт-09.03.03.02-11</t>
   </si>
   <si>
@@ -208,6 +172,24 @@
   </si>
   <si>
     <t>Кузнецова О.В.</t>
+  </si>
+  <si>
+    <t>понедельник</t>
+  </si>
+  <si>
+    <t>вторник</t>
+  </si>
+  <si>
+    <t>среда</t>
+  </si>
+  <si>
+    <t>четверг</t>
+  </si>
+  <si>
+    <t>пятница</t>
+  </si>
+  <si>
+    <t>суббота</t>
   </si>
 </sst>
 </file>
@@ -499,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -512,22 +494,22 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,7 +517,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,17 +525,17 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -561,7 +543,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,17 +551,17 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,7 +569,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,48 +577,48 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -644,7 +626,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -652,14 +634,14 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="7"/>
@@ -679,7 +661,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="7"/>
@@ -698,10 +680,10 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -718,11 +700,11 @@
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,7 +712,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -738,17 +720,17 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -756,7 +738,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,17 +746,17 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -782,7 +764,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -790,17 +772,17 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,7 +790,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,16 +798,16 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" s="7"/>
     </row>
@@ -833,7 +815,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="7"/>
     </row>
@@ -841,17 +823,17 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D41" s="7"/>
     </row>
@@ -859,7 +841,7 @@
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D42" s="7"/>
     </row>
@@ -867,20 +849,20 @@
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,7 +870,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -896,17 +878,17 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -914,7 +896,7 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -922,110 +904,110 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D59" s="7"/>
     </row>
@@ -1033,7 +1015,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D60" s="7"/>
     </row>
@@ -1041,14 +1023,14 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="7"/>
@@ -1067,14 +1049,14 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1082,7 +1064,7 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1090,17 +1072,17 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1108,7 +1090,7 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1116,77 +1098,77 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D74" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="7"/>
@@ -1206,7 +1188,7 @@
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="7"/>
@@ -1226,7 +1208,7 @@
     <row r="83" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="7"/>
@@ -1245,10 +1227,10 @@
     </row>
     <row r="86" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="7"/>
@@ -1268,11 +1250,11 @@
     <row r="89" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1280,7 +1262,7 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1288,17 +1270,17 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,7 +1288,7 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1314,48 +1296,48 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D98" s="7"/>
     </row>
@@ -1363,7 +1345,7 @@
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D99" s="7"/>
     </row>
@@ -1371,14 +1353,14 @@
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D100" s="7"/>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="7"/>
@@ -1398,7 +1380,7 @@
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="7"/>
@@ -1417,13 +1399,13 @@
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D107" s="7"/>
     </row>
@@ -1431,7 +1413,7 @@
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D108" s="7"/>
     </row>
@@ -1439,17 +1421,17 @@
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D109" s="7"/>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D110" s="7"/>
     </row>
@@ -1457,7 +1439,7 @@
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D111" s="7"/>
     </row>
@@ -1465,17 +1447,17 @@
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D112" s="7"/>
     </row>
     <row r="113" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D113" s="7"/>
     </row>
@@ -1483,7 +1465,7 @@
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D114" s="7"/>
     </row>
@@ -1491,17 +1473,17 @@
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D115" s="7"/>
     </row>
     <row r="116" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D116" s="7"/>
     </row>
@@ -1509,7 +1491,7 @@
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D117" s="7"/>
     </row>
@@ -1517,14 +1499,14 @@
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D118" s="7"/>
     </row>
     <row r="119" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="7"/>
@@ -1544,7 +1526,7 @@
     <row r="122" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="7"/>
@@ -1564,7 +1546,7 @@
     <row r="125" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="7"/>
@@ -2462,7 +2444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2472,22 +2456,22 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2495,7 +2479,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,17 +2487,17 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2521,7 +2505,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2529,17 +2513,17 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2547,7 +2531,7 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="7" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2555,48 +2539,48 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" s="7" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -2604,7 +2588,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -2612,14 +2596,14 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="7"/>
@@ -2639,7 +2623,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
@@ -2658,10 +2642,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -2678,11 +2662,11 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2690,7 +2674,7 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2698,17 +2682,17 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,7 +2700,7 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="7" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,17 +2708,17 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="7" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2742,7 +2726,7 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2750,17 +2734,17 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,7 +2752,7 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2776,13 +2760,13 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="7"/>
@@ -2802,7 +2786,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="7"/>
@@ -2821,14 +2805,14 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,7 +2820,7 @@
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,17 +2828,17 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="7" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2862,7 +2846,7 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,110 +2854,110 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D59" s="7"/>
     </row>
@@ -2981,7 +2965,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D60" s="7"/>
     </row>
@@ -2989,14 +2973,14 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="7"/>
@@ -3015,14 +2999,14 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3030,7 +3014,7 @@
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,17 +3022,17 @@
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3056,7 +3040,7 @@
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3064,77 +3048,77 @@
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="D74" s="7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="7"/>
@@ -3154,7 +3138,7 @@
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="7"/>
@@ -3174,7 +3158,7 @@
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="7"/>
@@ -3193,10 +3177,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="7"/>
@@ -3216,7 +3200,7 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="7"/>
@@ -3236,7 +3220,7 @@
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="7"/>
@@ -3256,7 +3240,7 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="7"/>
@@ -3276,7 +3260,7 @@
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="7"/>
@@ -3296,7 +3280,7 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="7"/>
@@ -3316,7 +3300,7 @@
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="7"/>
@@ -3335,13 +3319,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D107" s="7"/>
     </row>
@@ -3349,7 +3333,7 @@
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D108" s="7"/>
     </row>
@@ -3357,17 +3341,17 @@
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D109" s="7"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D110" s="7"/>
     </row>
@@ -3375,7 +3359,7 @@
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D111" s="7"/>
     </row>
@@ -3383,17 +3367,17 @@
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D112" s="7"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D113" s="7"/>
     </row>
@@ -3401,7 +3385,7 @@
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D114" s="7"/>
     </row>
@@ -3409,17 +3393,17 @@
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D115" s="7"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D116" s="7"/>
     </row>
@@ -3427,7 +3411,7 @@
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D117" s="7"/>
     </row>
@@ -3435,14 +3419,14 @@
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D118" s="7"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C119" s="3"/>
       <c r="D119" s="7"/>
@@ -3462,7 +3446,7 @@
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="7"/>
@@ -3482,7 +3466,7 @@
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C125" s="3"/>
       <c r="D125" s="7"/>

</xml_diff>